<commit_message>
files with all scores
</commit_message>
<xml_diff>
--- a/training_features/2024-11-14_11-39-15/scores_llama3.1_8b_0-shot_500.xlsx
+++ b/training_features/2024-11-14_11-39-15/scores_llama3.1_8b_0-shot_500.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,30 +446,45 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>LR-mse</t>
+          <t>ridge-mse</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>LR-mae</t>
+          <t>ridge-mae</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>LR-r2</t>
+          <t>ridge-r2</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>lasso-mse</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>lasso-mae</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>lasso-r2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>xgboost-mse</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>xgboost-mae</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>xgboost-r2</t>
         </is>
@@ -488,22 +503,31 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.272738525030661</v>
+        <v>0.4555217868538914</v>
       </c>
       <c r="E2" t="n">
-        <v>1.001021087635301</v>
+        <v>0.6559421920886156</v>
       </c>
       <c r="F2" t="n">
-        <v>-99.94955297510916</v>
+        <v>0.4089549219551496</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.4895832612129138</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.6329498048539489</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.3647597432571255</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.9941698772103497</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.8569269179105919</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-0.289947509765625</v>
       </c>
     </row>
     <row r="3">
@@ -519,22 +543,31 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.004681242366835372</v>
+        <v>0.002988124313379409</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06599712985192831</v>
+        <v>0.04841758608595412</v>
       </c>
       <c r="F3" t="n">
-        <v>-9.58182421104091</v>
+        <v>-5.725437550555314</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.0004651032234788107</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.01966173521066257</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>-0.04681812268080887</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0002132211573344991</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.01115800543319008</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.5200984477996826</v>
       </c>
     </row>
     <row r="4">
@@ -550,22 +583,31 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1479965668163936</v>
+        <v>0.7389480115939605</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3383179479787091</v>
+        <v>0.7090462086306203</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2664054963559134</v>
+        <v>-1.008301059448199</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1.054001041272581</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.8333021419539891</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>-1.864547132728939</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.270454786461915</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.4414485555339542</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.2649623155593872</v>
       </c>
     </row>
     <row r="5">
@@ -581,22 +623,31 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.0300243437951129</v>
+        <v>0.02066471219480738</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1460974739833959</v>
+        <v>0.1250926694518139</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.5467061950609207</v>
+        <v>-3.539807495611556</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.004580809464952993</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.06032313217986614</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>-0.006352904841692819</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.02385738694551365</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1367146381495341</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-4.241201877593994</v>
       </c>
     </row>
     <row r="6">
@@ -612,22 +663,31 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.4119446936554683</v>
+        <v>0.1802190135412876</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6088141651301388</v>
+        <v>0.317837250480989</v>
       </c>
       <c r="F6" t="n">
-        <v>0.175995270033151</v>
+        <v>0.6583704394415938</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.1386172118951059</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.2841927836159081</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.7372322916710037</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.07918632673914</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.6152668863188908</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-1.045743703842163</v>
       </c>
     </row>
     <row r="7">
@@ -643,22 +703,31 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.007102389845688404</v>
+        <v>0.003913098349716283</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05975895530742376</v>
+        <v>0.04928439693972672</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.05220876232568683</v>
+        <v>-9.760130853583744</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.0006548470085674035</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>0.01880624568997617</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>-0.800680399912264</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.01509386526502207</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1099542017857684</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-40.50469970703125</v>
       </c>
     </row>
     <row r="8">
@@ -674,22 +743,31 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.03688144417944873</v>
+        <v>0.02175824278738109</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1827001729182579</v>
+        <v>0.120872224357004</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8165015843196424</v>
+        <v>0.919725851458979</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>0.1320598131212355</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.3278540909346548</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>0.5127828493143907</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.685048653619287</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.614575346711288</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1.527396202087402</v>
       </c>
     </row>
     <row r="9">
@@ -705,22 +783,31 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.03418111233205287</v>
+        <v>0.03528139083177481</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1612641338237301</v>
+        <v>0.1629928061165129</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3873604781714681</v>
+        <v>0.1955535449817951</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.04882442177626456</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.1789632000866924</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>-0.1132393618920686</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.06474638960879475</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.1706129851657544</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.4762741327285767</v>
       </c>
     </row>
     <row r="10">
@@ -736,22 +823,31 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.2773095619341656</v>
+        <v>0.2165676706663755</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4519167710088678</v>
+        <v>0.3850714572422671</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4138175195565893</v>
+        <v>0.6478062969415443</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>0.2169920778858596</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>0.4002062236725769</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.6471161036648891</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.01612003466364265</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.1100539504757916</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.9737847447395325</v>
       </c>
     </row>
     <row r="11">
@@ -767,22 +863,31 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.006772592443601781</v>
+        <v>0.002904497425419079</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06320780968964818</v>
+        <v>0.04561174881337166</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4017142641314676</v>
+        <v>-0.7131849952988543</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.001980770454537891</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>0.03633533443243084</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>-0.168335076542883</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.001224997556019624</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.02975516769273273</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.2774490714073181</v>
       </c>
     </row>
     <row r="12">
@@ -798,22 +903,31 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.01450296874786915</v>
+        <v>0.01829065190554527</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1137936812231353</v>
+        <v>0.1295127589827779</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9773860114693936</v>
+        <v>0.9713119060660635</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.1758797151961127</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.4028342615075391</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.7241402976407667</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.559754919707975</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9109831966430725</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-1.446408033370972</v>
       </c>
     </row>
     <row r="13">
@@ -829,22 +943,31 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.02941400572824437</v>
+        <v>0.006238006300636372</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1438756321681871</v>
+        <v>0.07542658245285325</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.6604576690017467</v>
+        <v>0.697598906782974</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>0.02101479259695365</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>0.120973362300728</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>-0.01873835145045488</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.01618400814564043</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.1117747390547664</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.2154445648193359</v>
       </c>
     </row>
     <row r="14">
@@ -860,22 +983,31 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.12981972546352</v>
+        <v>0.1281430031346213</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3089349389142809</v>
+        <v>0.3020507033891499</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.1109718385714873</v>
+        <v>0.589641172113655</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.1093031179273313</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.2328201897832586</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.649973090533382</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.1285136656382808</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.2434322092452112</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.5884541273117065</v>
       </c>
     </row>
     <row r="15">
@@ -891,22 +1023,31 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.002918620621624469</v>
+        <v>0.005768714101245766</v>
       </c>
       <c r="E15" t="n">
-        <v>0.04545875049633528</v>
+        <v>0.06019330579646735</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4285737619776644</v>
+        <v>0.2888615355659494</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>0.008806101573942914</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>0.07226114276315541</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>-0.08557252812921878</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.005505576747574583</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.06214438497687997</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.3212997317314148</v>
       </c>
     </row>
     <row r="16">
@@ -922,22 +1063,31 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.00518879360794411</v>
+        <v>0.005381720170851961</v>
       </c>
       <c r="E16" t="n">
-        <v>0.06047981593149613</v>
+        <v>0.0667412693438502</v>
       </c>
       <c r="F16" t="n">
-        <v>0.988768198851977</v>
+        <v>0.9898084578963992</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>0.05331054510796161</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>0.1769343105197016</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>0.8990440513840965</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.06454078295409384</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.2003400080982035</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.8777769804000854</v>
       </c>
     </row>
     <row r="17">
@@ -953,22 +1103,31 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.02220188139115934</v>
+        <v>0.01420746769981548</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1208244515043594</v>
+        <v>0.09014339940749733</v>
       </c>
       <c r="F17" t="n">
-        <v>0.130401081914439</v>
+        <v>0.5046880225955535</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>0.0299519725747963</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>0.1386325015044186</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>-0.04420936064340197</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.01667851580566424</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.1065035275297454</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.4185404181480408</v>
       </c>
     </row>
     <row r="18">
@@ -984,22 +1143,31 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.5281657182203853</v>
+        <v>0.429715549898142</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5848875346415494</v>
+        <v>0.5351080393155605</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2026473694444251</v>
+        <v>0.5477588934265191</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.5402706405748542</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>0.5762972430694974</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.4314085389726972</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1656705155254224</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.2680925709018356</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.8256450891494751</v>
       </c>
     </row>
     <row r="19">
@@ -1015,22 +1183,31 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.006515414507673701</v>
+        <v>0.003192438265960879</v>
       </c>
       <c r="E19" t="n">
-        <v>0.06560869567986889</v>
+        <v>0.04665420423086466</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6138337445865136</v>
+        <v>0.7843873761292298</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.01638856303714907</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>0.08784196247361803</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>-0.1068596425458737</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.003327193912451756</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.04732199711247242</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.7752861976623535</v>
       </c>
     </row>
     <row r="20">
@@ -1046,22 +1223,31 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.002965034728832181</v>
+        <v>0.0009082024813792507</v>
       </c>
       <c r="E20" t="n">
-        <v>0.04727710996062549</v>
+        <v>0.02407132256367746</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9930158691291312</v>
+        <v>0.9984369481081193</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>0.05153392827035109</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>0.188901391640382</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>0.9113080995366933</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.1195801711162124</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.2250336787862857</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.7941978573799133</v>
       </c>
     </row>
     <row r="21">
@@ -1077,22 +1263,31 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.0127300496885489</v>
+        <v>0.01836915555100058</v>
       </c>
       <c r="E21" t="n">
-        <v>0.08357832313435669</v>
+        <v>0.1063966136919262</v>
       </c>
       <c r="F21" t="n">
-        <v>0.323560742790207</v>
+        <v>0.2427956669827205</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>0.02571000984740296</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>0.113159588073467</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>-0.0598054333156337</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.01450148985258233</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.1002564532156792</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.4022267460823059</v>
       </c>
     </row>
     <row r="22">
@@ -1108,22 +1303,31 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.3055308737072618</v>
+        <v>0.2954145445497295</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4302499734727361</v>
+        <v>0.4277541684096843</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4877872360456642</v>
+        <v>0.3751370817637872</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.2703131541825919</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>0.4187001343823662</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>0.4282317188626575</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.2026646684747554</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.3225759123778066</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.5713223218917847</v>
       </c>
     </row>
     <row r="23">
@@ -1139,22 +1343,31 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.005003254049543266</v>
+        <v>0.002089291442636698</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05336481439588318</v>
+        <v>0.03201062185616397</v>
       </c>
       <c r="F23" t="n">
-        <v>0.7771322023647058</v>
+        <v>0.702512701093067</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>0.007079411729769635</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.05803782232839373</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>-0.008014023491810685</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.001998942698850641</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.0310712653184708</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.715377151966095</v>
       </c>
     </row>
     <row r="24">
@@ -1170,22 +1383,31 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.002937908051578546</v>
+        <v>0.0007908554371018908</v>
       </c>
       <c r="E24" t="n">
-        <v>0.04618588500753187</v>
+        <v>0.02523672238464457</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9888672536310429</v>
+        <v>0.9989407170998003</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>0.04942457013328184</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>0.1919306277113631</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>0.9338000353341934</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.03019950871981471</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.113530555891872</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.9595503807067871</v>
       </c>
     </row>
     <row r="25">
@@ -1201,22 +1423,31 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.02692706060762063</v>
+        <v>0.02619433802044649</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1211425276495143</v>
+        <v>0.1280007366101777</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.5922152530897533</v>
+        <v>0.3656375753349544</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>0.04459541574564238</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>0.1607998004004359</v>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>-0.07999125762481274</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0243807035184296</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.1143278450541323</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.4095593690872192</v>
       </c>
     </row>
     <row r="26">
@@ -1232,22 +1463,31 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.3507793512613079</v>
+        <v>0.5918112836059127</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4557659006540961</v>
+        <v>0.6565435249110751</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5230053525479866</v>
+        <v>0.1893538713534353</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>0.5730060388032903</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>0.6323304162728374</v>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>0.2151127565247563</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.2009062157758014</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.347596522544342</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.7248044013977051</v>
       </c>
     </row>
     <row r="27">
@@ -1263,22 +1503,31 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.002483774619414013</v>
+        <v>0.003389784043762349</v>
       </c>
       <c r="E27" t="n">
-        <v>0.03953642951592836</v>
+        <v>0.04810297724058742</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7307866910765939</v>
+        <v>0.7998404419569527</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.0198941962348144</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>0.104107163553916</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>-0.1747100920218019</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.001684586643748755</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.03282225607969128</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.9005287289619446</v>
       </c>
     </row>
     <row r="28">
@@ -1294,22 +1543,31 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.001545406261228</v>
+        <v>0.0007378768616483174</v>
       </c>
       <c r="E28" t="n">
-        <v>0.03047544670360625</v>
+        <v>0.02282283350922887</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9961885841296393</v>
+        <v>0.9980035076043899</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.06072601871421245</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>0.2066465479201345</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>0.8356920498797482</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01835511858529847</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.09758033056552942</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.9503360986709595</v>
       </c>
     </row>
     <row r="29">
@@ -1325,22 +1583,31 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.01305958332568587</v>
+        <v>0.008211769075595713</v>
       </c>
       <c r="E29" t="n">
-        <v>0.09776919746165286</v>
+        <v>0.07057391302081108</v>
       </c>
       <c r="F29" t="n">
-        <v>0.4444128269325514</v>
+        <v>0.4221758628744071</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.01427557615828159</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>0.09460049682468691</v>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>-0.004506142305438443</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0.002965972668589699</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.04715802334407618</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.7912982702255249</v>
       </c>
     </row>
     <row r="30">
@@ -1356,22 +1623,31 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.7149814397654978</v>
+        <v>0.4976319942844214</v>
       </c>
       <c r="E30" t="n">
-        <v>0.6527180242584451</v>
+        <v>0.5705188146567043</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.03795842599114385</v>
+        <v>0.4206011821853636</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>0.5672802520990349</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>0.5944915056872853</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.3395088916893234</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0.3608427712787368</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.4130952286648139</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.5798665285110474</v>
       </c>
     </row>
     <row r="31">
@@ -1387,22 +1663,31 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.002020773571423674</v>
+        <v>0.002520021092827574</v>
       </c>
       <c r="E31" t="n">
-        <v>0.03686864350218162</v>
+        <v>0.04294386817466987</v>
       </c>
       <c r="F31" t="n">
-        <v>0.7470455802538407</v>
+        <v>0.7914540186794278</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>0.01282972360056906</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.07336148684526496</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>-0.06173210453181377</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.0011873180670401</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.02754906872393228</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.9017427563667297</v>
       </c>
     </row>
     <row r="32">
@@ -1418,22 +1703,31 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.0006212165520109686</v>
+        <v>0.0004529305633722731</v>
       </c>
       <c r="E32" t="n">
-        <v>0.02103451229773954</v>
+        <v>0.01579541117688398</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9989543942224978</v>
+        <v>0.9992365225234001</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.05768198761653275</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.1843763734208168</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>0.9027689851114311</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.03881342973865676</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.1317587647781326</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.9345745444297791</v>
       </c>
     </row>
     <row r="33">
@@ -1449,22 +1743,31 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.03097975634949345</v>
+        <v>0.02690364466051384</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1327099562315243</v>
+        <v>0.1262348938064764</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.2394496935559249</v>
+        <v>0.3420724965303507</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>0.04099381087767926</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>0.1566502833858486</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>-0.002501928225487893</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.002311185659356185</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.03963498097968482</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.9434800744056702</v>
       </c>
     </row>
     <row r="34">
@@ -1480,22 +1783,31 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.9610149136020211</v>
+        <v>0.7432741230166445</v>
       </c>
       <c r="E34" t="n">
-        <v>0.7610706765292633</v>
+        <v>0.677410285073865</v>
       </c>
       <c r="F34" t="n">
-        <v>0.2455866242951121</v>
+        <v>-0.1084399780585281</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>0.6958140768215628</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>0.647586677766791</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>-0.03766311265438294</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.4693920920131764</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.4531089294904214</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.2999984622001648</v>
       </c>
     </row>
     <row r="35">
@@ -1511,22 +1823,31 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.003266737125740131</v>
+        <v>0.0040338970416183</v>
       </c>
       <c r="E35" t="n">
-        <v>0.04611816295950109</v>
+        <v>0.04861330311805478</v>
       </c>
       <c r="F35" t="n">
-        <v>0.8102455383377797</v>
+        <v>0.7938000717156422</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>0.01961147848968805</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>0.1081032368923594</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>-0.00247612083366322</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.001731022700665793</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.029252196112437</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.9115156531333923</v>
       </c>
     </row>
     <row r="36">
@@ -1542,22 +1863,31 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.000383843834156819</v>
+        <v>0.0004381527215155775</v>
       </c>
       <c r="E36" t="n">
-        <v>0.01561489597329374</v>
+        <v>0.01727574288092266</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9991744604090941</v>
+        <v>0.9991789886652012</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>0.04092186012248861</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>0.1691207425407663</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>0.9233205470334578</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.01498235216580923</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.07894558452209127</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.9719260334968567</v>
       </c>
     </row>
     <row r="37">
@@ -1573,22 +1903,31 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.01489578736157146</v>
+        <v>0.02613547158090934</v>
       </c>
       <c r="E37" t="n">
-        <v>0.08772046660108747</v>
+        <v>0.1143382813535579</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5365869293904399</v>
+        <v>0.4242269286562712</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>0.04828291257090975</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>0.1596333759790792</v>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>-0.06368851154306165</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0.008917237488669851</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.06287509041528928</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0.8035502433776855</v>
       </c>
     </row>
     <row r="38">
@@ -1604,22 +1943,31 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.6360998757536743</v>
+        <v>0.6987028627198645</v>
       </c>
       <c r="E38" t="n">
-        <v>0.671408877849263</v>
+        <v>0.689576246984151</v>
       </c>
       <c r="F38" t="n">
-        <v>0.5611313604297692</v>
+        <v>0.5232675613674</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>0.7149922521956358</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>0.7021636212667907</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>0.5121531366484416</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.2369010373415994</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.3659951379019186</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.8383598923683167</v>
       </c>
     </row>
     <row r="39">
@@ -1635,22 +1983,31 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.002126034093291866</v>
+        <v>0.002149682634554463</v>
       </c>
       <c r="E39" t="n">
-        <v>0.03470775531211121</v>
+        <v>0.03630753474199502</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6560754727590548</v>
+        <v>0.8432058151066411</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>0.01416858840960472</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>0.09288755833181378</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>-0.03343267283447071</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0.001013591582794082</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.0241912983721007</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.9260703325271606</v>
       </c>
     </row>
     <row r="40">
@@ -1666,22 +2023,31 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.0003125645248692131</v>
+        <v>0.0003866574697316616</v>
       </c>
       <c r="E40" t="n">
-        <v>0.01369428965736787</v>
+        <v>0.01554053245105381</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9995452634539188</v>
+        <v>0.9993528980844308</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>0.03153958269424816</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>0.1435281012870241</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.947216009063882</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0.04104149805828988</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.1479359758981671</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0.9313138127326965</v>
       </c>
     </row>
     <row r="41">
@@ -1697,22 +2063,31 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.01104147724073007</v>
+        <v>0.02345862545883696</v>
       </c>
       <c r="E41" t="n">
-        <v>0.07676686334984389</v>
+        <v>0.1068870127110012</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5813658932358796</v>
+        <v>0.425593946493137</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>0.04728331565394796</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>0.1634508183448903</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>-0.1577755392855853</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0.005540338678735042</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.05303952676454876</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0.8643397092819214</v>
       </c>
     </row>
     <row r="42">
@@ -1728,22 +2103,31 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.5707275539500788</v>
+        <v>0.8829465774625439</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5963080765453487</v>
+        <v>0.7718022041906407</v>
       </c>
       <c r="F42" t="n">
-        <v>0.20623444485733</v>
+        <v>0.1648456019557372</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>0.7698737354345889</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>0.7099937863494876</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>0.2717980311620408</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.4615475742106706</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.4378278312754901</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0.5634350776672363</v>
       </c>
     </row>
     <row r="43">
@@ -1759,22 +2143,31 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.001840249632563301</v>
+        <v>0.003257710828626241</v>
       </c>
       <c r="E43" t="n">
-        <v>0.03676928262432123</v>
+        <v>0.04888762447656634</v>
       </c>
       <c r="F43" t="n">
-        <v>0.8781893702421425</v>
+        <v>0.8448899972503131</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>0.02103183829883955</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>0.1192327957034324</v>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>-0.001392900713549361</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.001207541261561012</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.0229813967426578</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.9425051212310791</v>
       </c>
     </row>
     <row r="44">
@@ -1790,22 +2183,31 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.0002018366131182123</v>
+        <v>0.0003714879565056171</v>
       </c>
       <c r="E44" t="n">
-        <v>0.01135675062104692</v>
+        <v>0.01576981514940986</v>
       </c>
       <c r="F44" t="n">
-        <v>0.9996402804034157</v>
+        <v>0.9994360003434568</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>0.04716679962838002</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>0.1845209071396596</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.9283905216177682</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0.02592102022334339</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.1193012027367688</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.9606462717056274</v>
       </c>
     </row>
     <row r="45">
@@ -1821,22 +2223,31 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.01611974969238979</v>
+        <v>0.02537644589697369</v>
       </c>
       <c r="E45" t="n">
-        <v>0.09267787085470752</v>
+        <v>0.1227012247935206</v>
       </c>
       <c r="F45" t="n">
-        <v>0.3106412667192852</v>
+        <v>0.3783356222217132</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>0.04117650642544363</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>0.1613923439557332</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>-0.008729407970789582</v>
+      </c>
+      <c r="J45" t="n">
+        <v>0.01113764919293969</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0.06641011125885074</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0.7271532416343689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>